<commit_message>
Update spreadsheet column headings and include Wagga2008
</commit_message>
<xml_diff>
--- a/Prototypes/Canola/Greenethorpe2013.xlsx
+++ b/Prototypes/Canola/Greenethorpe2013.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lil026\ApsimX\Prototypes\Canola\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7433EC1-B876-4F9E-B0E6-10CBEF91C56D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA7F1F55-26BA-4FFB-94B8-C3717A2DEE70}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="4260" yWindow="4125" windowWidth="15210" windowHeight="15435" xr2:uid="{82FDB4BE-E74B-4488-8680-42A462D2A87F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{82FDB4BE-E74B-4488-8680-42A462D2A87F}"/>
   </bookViews>
   <sheets>
     <sheet name="Observed" sheetId="1" r:id="rId1"/>
@@ -83,42 +83,21 @@
     <t>Canola.Leaf.Dead.NConc</t>
   </si>
   <si>
-    <t>podwallNconc</t>
-  </si>
-  <si>
     <t>Canola.Stem.NConc</t>
   </si>
   <si>
     <t>Canola.Leaf.Live.Nconc</t>
   </si>
   <si>
-    <t>canola.Leaf.SpecificArea</t>
-  </si>
-  <si>
-    <t>Canola.density</t>
-  </si>
-  <si>
     <t>Canola.Leaf.LAI</t>
   </si>
   <si>
     <t>GrainsPerPod</t>
   </si>
   <si>
-    <t>Canola.grain.number</t>
-  </si>
-  <si>
-    <t>canola.pod.number</t>
-  </si>
-  <si>
-    <t>Canola.grain.wt</t>
-  </si>
-  <si>
     <t>Harvest_index</t>
   </si>
   <si>
-    <t>Canola.Grain.Total.Wt</t>
-  </si>
-  <si>
     <t>Canola.Leaf.Dead.Wt</t>
   </si>
   <si>
@@ -140,9 +119,6 @@
     <t>treat</t>
   </si>
   <si>
-    <t>Cultivar</t>
-  </si>
-  <si>
     <t>exp</t>
   </si>
   <si>
@@ -153,6 +129,30 @@
   </si>
   <si>
     <t>Canola.Stem.Wt</t>
+  </si>
+  <si>
+    <t>Canola.Cultivar</t>
+  </si>
+  <si>
+    <t>Canola.Grain.Wt</t>
+  </si>
+  <si>
+    <t>Canola.Grain.Size</t>
+  </si>
+  <si>
+    <t>Canola.Pod.Number</t>
+  </si>
+  <si>
+    <t>Canola.Grain.Number</t>
+  </si>
+  <si>
+    <t>Canola.Density</t>
+  </si>
+  <si>
+    <t>Canola.Leaf.SpecificArea</t>
+  </si>
+  <si>
+    <t>Canola.Shell.Nconc</t>
   </si>
 </sst>
 </file>
@@ -508,9 +508,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7873D758-2B96-4EE8-A7C0-7EBF4418075C}">
   <dimension ref="A1:Y29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -543,76 +541,76 @@
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>30</v>
+      </c>
+      <c r="R1" t="s">
+        <v>13</v>
+      </c>
+      <c r="S1" t="s">
+        <v>12</v>
+      </c>
+      <c r="T1" t="s">
+        <v>31</v>
+      </c>
+      <c r="U1" t="s">
         <v>32</v>
       </c>
-      <c r="B1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H1" t="s">
-        <v>25</v>
-      </c>
-      <c r="I1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="V1" t="s">
+        <v>11</v>
+      </c>
+      <c r="W1" t="s">
+        <v>10</v>
+      </c>
+      <c r="X1" t="s">
         <v>33</v>
-      </c>
-      <c r="K1" t="s">
-        <v>23</v>
-      </c>
-      <c r="L1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M1" t="s">
-        <v>21</v>
-      </c>
-      <c r="N1" t="s">
-        <v>20</v>
-      </c>
-      <c r="O1" t="s">
-        <v>19</v>
-      </c>
-      <c r="P1" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>17</v>
-      </c>
-      <c r="R1" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" t="s">
-        <v>15</v>
-      </c>
-      <c r="T1" t="s">
-        <v>14</v>
-      </c>
-      <c r="U1" t="s">
-        <v>13</v>
-      </c>
-      <c r="V1" t="s">
-        <v>12</v>
-      </c>
-      <c r="W1" t="s">
-        <v>11</v>
-      </c>
-      <c r="X1" t="s">
-        <v>10</v>
       </c>
       <c r="Y1" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
updated parameter names for phenology
</commit_message>
<xml_diff>
--- a/Prototypes/Canola/Greenethorpe2013.xlsx
+++ b/Prototypes/Canola/Greenethorpe2013.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lil026\ApsimX\Prototypes\Canola\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA7F1F55-26BA-4FFB-94B8-C3717A2DEE70}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5EA82CF-B5D3-46A2-8AF2-E08E94414395}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{82FDB4BE-E74B-4488-8680-42A462D2A87F}"/>
   </bookViews>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="36">
   <si>
     <t>uncut</t>
   </si>
@@ -153,6 +153,12 @@
   </si>
   <si>
     <t>Canola.Shell.Nconc</t>
+  </si>
+  <si>
+    <t>Canola.DaysAfterSowing</t>
+  </si>
+  <si>
+    <t>Canola.Stage</t>
   </si>
 </sst>
 </file>
@@ -188,10 +194,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -506,9 +513,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7873D758-2B96-4EE8-A7C0-7EBF4418075C}">
-  <dimension ref="A1:Y29"/>
+  <dimension ref="A1:AA29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -519,27 +528,29 @@
     <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.7109375" customWidth="1"/>
-    <col min="12" max="12" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="23" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" customWidth="1"/>
+    <col min="9" max="9" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5703125" customWidth="1"/>
+    <col min="11" max="11" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.7109375" customWidth="1"/>
+    <col min="14" max="14" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="23" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="22.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -562,63 +573,69 @@
         <v>19</v>
       </c>
       <c r="H1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" t="s">
         <v>18</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" t="s">
         <v>17</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>25</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>16</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>15</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>27</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>28</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>29</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>30</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>13</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>12</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>31</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>32</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>11</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>10</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
         <v>33</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AA1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
-        <f t="shared" ref="A2:A29" si="0">B2&amp;H2&amp;C2&amp;"Cv"&amp;D2</f>
+        <f t="shared" ref="A2:A29" si="0">B2&amp;I2&amp;C2&amp;"Cv"&amp;D2</f>
         <v>Greenethorpe2013_Ex1CvHyola971_CL</v>
       </c>
       <c r="B2" t="s">
@@ -639,29 +656,33 @@
       <c r="G2" s="1">
         <v>41401</v>
       </c>
-      <c r="H2">
-        <v>2013</v>
+      <c r="H2" s="3">
+        <f>G2-F2</f>
+        <v>43</v>
       </c>
       <c r="I2">
+        <v>2013</v>
+      </c>
+      <c r="K2">
         <v>123.7843249</v>
       </c>
-      <c r="J2">
+      <c r="L2">
         <v>24.714967470000001</v>
       </c>
-      <c r="K2">
+      <c r="M2">
         <v>89.599000000000004</v>
       </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="S2">
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="U2">
         <v>1.52</v>
       </c>
-      <c r="U2">
+      <c r="W2">
         <v>169.28</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex1CvHyola971_CL</v>
@@ -684,29 +705,33 @@
       <c r="G3" s="1">
         <v>41444</v>
       </c>
-      <c r="H3">
-        <v>2013</v>
+      <c r="H3" s="3">
+        <f t="shared" ref="H3:H29" si="1">G3-F3</f>
+        <v>86</v>
       </c>
       <c r="I3">
+        <v>2013</v>
+      </c>
+      <c r="K3">
         <v>429.71497690000001</v>
       </c>
-      <c r="J3">
+      <c r="L3">
         <v>200.63079859999999</v>
       </c>
-      <c r="K3">
+      <c r="M3">
         <v>163.90899999999999</v>
       </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-      <c r="S3">
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="U3">
         <v>3.42</v>
       </c>
-      <c r="U3">
+      <c r="W3">
         <v>207.81</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex1CvHyola971_CL</v>
@@ -729,32 +754,36 @@
       <c r="G4" s="1">
         <v>41479</v>
       </c>
-      <c r="H4">
-        <v>2013</v>
+      <c r="H4" s="3">
+        <f t="shared" si="1"/>
+        <v>121</v>
       </c>
       <c r="I4">
+        <v>2013</v>
+      </c>
+      <c r="K4">
         <v>539.07175570000004</v>
       </c>
-      <c r="J4">
+      <c r="L4">
         <v>278.7403248</v>
       </c>
-      <c r="K4">
+      <c r="M4">
         <v>217.08</v>
       </c>
-      <c r="L4">
+      <c r="N4">
         <v>43.252000000000002</v>
       </c>
-      <c r="S4">
+      <c r="U4">
         <v>3.97</v>
       </c>
-      <c r="T4">
+      <c r="V4">
         <v>41</v>
       </c>
-      <c r="U4">
+      <c r="W4">
         <v>182.68</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex1CvHyola971_CL</v>
@@ -777,32 +806,36 @@
       <c r="G5" s="1">
         <v>41492</v>
       </c>
-      <c r="H5">
-        <v>2013</v>
+      <c r="H5" s="3">
+        <f t="shared" si="1"/>
+        <v>134</v>
       </c>
       <c r="I5">
+        <v>2013</v>
+      </c>
+      <c r="K5">
         <v>720.40517309999996</v>
       </c>
-      <c r="J5">
+      <c r="L5">
         <v>398.96878989999999</v>
       </c>
-      <c r="K5">
+      <c r="M5">
         <v>213.77099999999999</v>
       </c>
-      <c r="L5">
+      <c r="N5">
         <v>107.66500000000001</v>
       </c>
-      <c r="S5">
+      <c r="U5">
         <v>4.4400000000000004</v>
       </c>
-      <c r="T5">
+      <c r="V5">
         <v>43</v>
       </c>
-      <c r="U5">
+      <c r="W5">
         <v>206.06</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex1CvHyola971_CL</v>
@@ -825,32 +858,36 @@
       <c r="G6" s="1">
         <v>41528</v>
       </c>
-      <c r="H6">
-        <v>2013</v>
+      <c r="H6" s="3">
+        <f t="shared" si="1"/>
+        <v>170</v>
       </c>
       <c r="I6">
+        <v>2013</v>
+      </c>
+      <c r="K6">
         <v>1325.831872</v>
       </c>
-      <c r="J6">
+      <c r="L6">
         <v>1037.2265259999999</v>
       </c>
-      <c r="K6">
+      <c r="M6">
         <v>185.126</v>
       </c>
-      <c r="L6">
+      <c r="N6">
         <v>103.479</v>
       </c>
-      <c r="S6">
+      <c r="U6">
         <v>2.96</v>
       </c>
-      <c r="T6">
+      <c r="V6">
         <v>37</v>
       </c>
-      <c r="U6">
+      <c r="W6">
         <v>158.69</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex1CvHyola971_CL</v>
@@ -873,29 +910,33 @@
       <c r="G7" s="1">
         <v>41563</v>
       </c>
-      <c r="H7">
-        <v>2013</v>
+      <c r="H7" s="3">
+        <f t="shared" si="1"/>
+        <v>205</v>
       </c>
       <c r="I7">
+        <v>2013</v>
+      </c>
+      <c r="K7">
         <v>961.09308520000002</v>
       </c>
-      <c r="J7">
+      <c r="L7">
         <v>674.67277030000002</v>
       </c>
-      <c r="K7">
+      <c r="M7">
         <v>9.2530000000000001</v>
       </c>
-      <c r="L7">
-        <v>0</v>
-      </c>
-      <c r="S7">
-        <v>0</v>
-      </c>
-      <c r="T7">
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="U7">
+        <v>0</v>
+      </c>
+      <c r="V7">
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex1CvHyola971_CL</v>
@@ -918,47 +959,54 @@
       <c r="G8" s="1">
         <v>41582</v>
       </c>
-      <c r="H8">
-        <v>2013</v>
+      <c r="H8" s="3">
+        <f t="shared" si="1"/>
+        <v>224</v>
       </c>
       <c r="I8">
+        <v>2013</v>
+      </c>
+      <c r="J8">
+        <v>9</v>
+      </c>
+      <c r="K8">
         <v>989.2505721</v>
       </c>
-      <c r="J8">
+      <c r="L8">
         <v>558.79506409999999</v>
       </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8">
-        <v>0</v>
-      </c>
       <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
         <v>279.39800000000002</v>
       </c>
-      <c r="N8">
+      <c r="P8">
         <v>0.28199999999999997</v>
       </c>
-      <c r="O8">
+      <c r="Q8">
         <v>4.0250000000000004</v>
       </c>
-      <c r="P8">
+      <c r="R8">
         <v>1360.933</v>
       </c>
-      <c r="Q8">
+      <c r="S8">
         <v>69733.97</v>
       </c>
-      <c r="R8">
+      <c r="T8">
         <v>52.042000000000002</v>
       </c>
-      <c r="S8">
-        <v>0</v>
-      </c>
-      <c r="T8">
+      <c r="U8">
+        <v>0</v>
+      </c>
+      <c r="V8">
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex2CvHyola_575_CL_GT</v>
@@ -981,14 +1029,18 @@
       <c r="G9" s="1">
         <v>41470</v>
       </c>
-      <c r="H9">
-        <v>2013</v>
+      <c r="H9" s="3">
+        <f t="shared" si="1"/>
+        <v>83</v>
       </c>
       <c r="I9">
+        <v>2013</v>
+      </c>
+      <c r="K9">
         <v>90.704614800000002</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex2CvHyola_575_CL_GT</v>
@@ -1011,32 +1063,36 @@
       <c r="G10" s="1">
         <v>41479</v>
       </c>
-      <c r="H10">
-        <v>2013</v>
+      <c r="H10" s="3">
+        <f t="shared" si="1"/>
+        <v>92</v>
       </c>
       <c r="I10">
+        <v>2013</v>
+      </c>
+      <c r="K10">
         <v>134.62814650000001</v>
       </c>
-      <c r="J10">
+      <c r="L10">
         <v>46.33188689</v>
       </c>
-      <c r="K10">
+      <c r="M10">
         <v>83.561999999999998</v>
       </c>
-      <c r="L10">
+      <c r="N10">
         <v>4.734</v>
       </c>
-      <c r="S10">
+      <c r="U10">
         <v>2.15</v>
       </c>
-      <c r="T10">
+      <c r="V10">
         <v>42</v>
       </c>
-      <c r="U10">
+      <c r="W10">
         <v>251.83</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex2CvHyola_575_CL_GT</v>
@@ -1059,32 +1115,36 @@
       <c r="G11" s="1">
         <v>41485</v>
       </c>
-      <c r="H11">
-        <v>2013</v>
+      <c r="H11" s="3">
+        <f t="shared" si="1"/>
+        <v>98</v>
       </c>
       <c r="I11">
+        <v>2013</v>
+      </c>
+      <c r="K11">
         <v>212.23959199999999</v>
       </c>
-      <c r="J11">
+      <c r="L11">
         <v>94.794925079999999</v>
       </c>
-      <c r="K11">
+      <c r="M11">
         <v>113.931</v>
       </c>
-      <c r="L11">
+      <c r="N11">
         <v>3.5129999999999999</v>
       </c>
-      <c r="S11">
+      <c r="U11">
         <v>3.42</v>
       </c>
-      <c r="T11">
+      <c r="V11">
         <v>41</v>
       </c>
-      <c r="U11">
+      <c r="W11">
         <v>302.83999999999997</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex2CvHyola_575_CL_GT</v>
@@ -1107,32 +1167,36 @@
       <c r="G12" s="1">
         <v>41492</v>
       </c>
-      <c r="H12">
-        <v>2013</v>
+      <c r="H12" s="3">
+        <f t="shared" si="1"/>
+        <v>105</v>
       </c>
       <c r="I12">
+        <v>2013</v>
+      </c>
+      <c r="K12">
         <v>353.1258593</v>
       </c>
-      <c r="J12">
+      <c r="L12">
         <v>186.52026179999999</v>
       </c>
-      <c r="K12">
+      <c r="M12">
         <v>158.36099999999999</v>
       </c>
-      <c r="L12">
+      <c r="N12">
         <v>8.2449999999999992</v>
       </c>
-      <c r="S12">
+      <c r="U12">
         <v>4.51</v>
       </c>
-      <c r="T12">
+      <c r="V12">
         <v>38</v>
       </c>
-      <c r="U12">
+      <c r="W12">
         <v>286.22000000000003</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex2CvHyola_575_CL_GT</v>
@@ -1155,32 +1219,36 @@
       <c r="G13" s="1">
         <v>41515</v>
       </c>
-      <c r="H13">
-        <v>2013</v>
+      <c r="H13" s="3">
+        <f t="shared" si="1"/>
+        <v>128</v>
       </c>
       <c r="I13">
+        <v>2013</v>
+      </c>
+      <c r="K13">
         <v>693.79042830000003</v>
       </c>
-      <c r="J13">
+      <c r="L13">
         <v>538.15308279999999</v>
       </c>
-      <c r="K13">
+      <c r="M13">
         <v>127.95699999999999</v>
       </c>
-      <c r="L13">
+      <c r="N13">
         <v>27.68</v>
       </c>
-      <c r="S13">
+      <c r="U13">
         <v>2.75</v>
       </c>
-      <c r="T13">
+      <c r="V13">
         <v>35</v>
       </c>
-      <c r="U13">
+      <c r="W13">
         <v>286.04000000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex2CvHyola_575_CL_GT</v>
@@ -1203,47 +1271,54 @@
       <c r="G14" s="1">
         <v>41570</v>
       </c>
-      <c r="H14">
-        <v>2013</v>
+      <c r="H14" s="3">
+        <f t="shared" si="1"/>
+        <v>183</v>
       </c>
       <c r="I14">
+        <v>2013</v>
+      </c>
+      <c r="J14">
+        <v>9</v>
+      </c>
+      <c r="K14">
         <v>1067.9271550000001</v>
       </c>
-      <c r="J14">
+      <c r="L14">
         <v>544.69423979999999</v>
       </c>
-      <c r="K14">
-        <v>0</v>
-      </c>
-      <c r="L14">
-        <v>0</v>
-      </c>
       <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
         <v>281.60000000000002</v>
       </c>
-      <c r="N14">
+      <c r="P14">
         <v>0.26300000000000001</v>
       </c>
-      <c r="O14">
+      <c r="Q14">
         <v>3.3069999999999999</v>
       </c>
-      <c r="P14">
+      <c r="R14">
         <v>3101.5940000000001</v>
       </c>
-      <c r="Q14">
+      <c r="S14">
         <v>85328.501000000004</v>
       </c>
-      <c r="R14">
+      <c r="T14">
         <v>27.488</v>
       </c>
-      <c r="S14">
-        <v>0</v>
-      </c>
-      <c r="T14">
+      <c r="U14">
+        <v>0</v>
+      </c>
+      <c r="V14">
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex3CvAV_Garnet</v>
@@ -1266,32 +1341,36 @@
       <c r="G15" s="1">
         <v>41479</v>
       </c>
-      <c r="H15">
-        <v>2013</v>
+      <c r="H15" s="3">
+        <f t="shared" si="1"/>
+        <v>92</v>
       </c>
       <c r="I15">
+        <v>2013</v>
+      </c>
+      <c r="K15">
         <v>101.8525934</v>
       </c>
-      <c r="J15">
+      <c r="L15">
         <v>36.962214240000002</v>
       </c>
-      <c r="K15">
+      <c r="M15">
         <v>63.087000000000003</v>
       </c>
-      <c r="L15">
+      <c r="N15">
         <v>1.8029999999999999</v>
       </c>
-      <c r="S15">
+      <c r="U15">
         <v>1.6</v>
       </c>
-      <c r="T15">
+      <c r="V15">
         <v>54</v>
       </c>
-      <c r="U15">
+      <c r="W15">
         <v>248.28</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex3CvCrusher_TT</v>
@@ -1314,32 +1393,36 @@
       <c r="G16" s="1">
         <v>41479</v>
       </c>
-      <c r="H16">
-        <v>2013</v>
+      <c r="H16" s="3">
+        <f t="shared" si="1"/>
+        <v>92</v>
       </c>
       <c r="I16">
+        <v>2013</v>
+      </c>
+      <c r="K16">
         <v>87.226353930000002</v>
       </c>
-      <c r="J16">
+      <c r="L16">
         <v>28.125936710000001</v>
       </c>
-      <c r="K16">
+      <c r="M16">
         <v>56.941000000000003</v>
       </c>
-      <c r="L16">
+      <c r="N16">
         <v>2.16</v>
       </c>
-      <c r="S16">
+      <c r="U16">
         <v>1.3</v>
       </c>
-      <c r="T16">
+      <c r="V16">
         <v>41</v>
       </c>
-      <c r="U16">
+      <c r="W16">
         <v>227.21</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex3CvHyola_575_CL_GT</v>
@@ -1362,32 +1445,36 @@
       <c r="G17" s="1">
         <v>41479</v>
       </c>
-      <c r="H17">
-        <v>2013</v>
+      <c r="H17" s="3">
+        <f t="shared" si="1"/>
+        <v>92</v>
       </c>
       <c r="I17">
+        <v>2013</v>
+      </c>
+      <c r="K17">
         <v>155.52345539999999</v>
       </c>
-      <c r="J17">
+      <c r="L17">
         <v>58.557161999999998</v>
       </c>
-      <c r="K17">
+      <c r="M17">
         <v>93.838999999999999</v>
       </c>
-      <c r="L17">
+      <c r="N17">
         <v>3.1269999999999998</v>
       </c>
-      <c r="S17">
+      <c r="U17">
         <v>2.37</v>
       </c>
-      <c r="T17">
+      <c r="V17">
         <v>43</v>
       </c>
-      <c r="U17">
+      <c r="W17">
         <v>253.76</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex3CvAV_Garnet</v>
@@ -1410,38 +1497,42 @@
       <c r="G18" s="1">
         <v>41485</v>
       </c>
-      <c r="H18">
-        <v>2013</v>
+      <c r="H18" s="3">
+        <f t="shared" si="1"/>
+        <v>98</v>
       </c>
       <c r="I18">
+        <v>2013</v>
+      </c>
+      <c r="K18">
         <v>162.50878030000001</v>
       </c>
-      <c r="J18">
+      <c r="L18">
         <v>64.736058679999999</v>
       </c>
-      <c r="K18">
+      <c r="M18">
         <v>92.834000000000003</v>
       </c>
-      <c r="L18">
+      <c r="N18">
         <v>4.9390000000000001</v>
       </c>
-      <c r="S18">
+      <c r="U18">
         <v>2.76</v>
       </c>
-      <c r="T18">
+      <c r="V18">
         <v>38</v>
       </c>
-      <c r="U18">
+      <c r="W18">
         <v>295.52</v>
       </c>
-      <c r="V18">
+      <c r="X18">
         <v>6.32</v>
       </c>
-      <c r="W18">
+      <c r="Y18">
         <v>5.16</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex3CvCrusher_TT</v>
@@ -1464,38 +1555,42 @@
       <c r="G19" s="1">
         <v>41485</v>
       </c>
-      <c r="H19">
-        <v>2013</v>
+      <c r="H19" s="3">
+        <f t="shared" si="1"/>
+        <v>98</v>
       </c>
       <c r="I19">
+        <v>2013</v>
+      </c>
+      <c r="K19">
         <v>118.0327194</v>
       </c>
-      <c r="J19">
+      <c r="L19">
         <v>46.828009399999999</v>
       </c>
-      <c r="K19">
+      <c r="M19">
         <v>67.88</v>
       </c>
-      <c r="L19">
+      <c r="N19">
         <v>3.3239999999999998</v>
       </c>
-      <c r="S19">
+      <c r="U19">
         <v>2.0699999999999998</v>
       </c>
-      <c r="T19">
+      <c r="V19">
         <v>39</v>
       </c>
-      <c r="U19">
+      <c r="W19">
         <v>304.13</v>
       </c>
-      <c r="V19">
+      <c r="X19">
         <v>6.66</v>
       </c>
-      <c r="W19">
+      <c r="Y19">
         <v>5.77</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex3CvHyola_575_CL_GT</v>
@@ -1518,38 +1613,42 @@
       <c r="G20" s="1">
         <v>41485</v>
       </c>
-      <c r="H20">
-        <v>2013</v>
+      <c r="H20" s="3">
+        <f t="shared" si="1"/>
+        <v>98</v>
       </c>
       <c r="I20">
+        <v>2013</v>
+      </c>
+      <c r="K20">
         <v>222.0954266</v>
       </c>
-      <c r="J20">
+      <c r="L20">
         <v>98.735454349999998</v>
       </c>
-      <c r="K20">
+      <c r="M20">
         <v>117.59699999999999</v>
       </c>
-      <c r="L20">
+      <c r="N20">
         <v>5.7629999999999999</v>
       </c>
-      <c r="S20">
+      <c r="U20">
         <v>3.57</v>
       </c>
-      <c r="T20">
+      <c r="V20">
         <v>50</v>
       </c>
-      <c r="U20">
+      <c r="W20">
         <v>306.02999999999997</v>
       </c>
-      <c r="V20">
+      <c r="X20">
         <v>6.53</v>
       </c>
-      <c r="W20">
+      <c r="Y20">
         <v>5.43</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex3CvAV_Garnet</v>
@@ -1572,41 +1671,45 @@
       <c r="G21" s="1">
         <v>41515</v>
       </c>
-      <c r="H21">
-        <v>2013</v>
+      <c r="H21" s="3">
+        <f t="shared" si="1"/>
+        <v>128</v>
       </c>
       <c r="I21">
+        <v>2013</v>
+      </c>
+      <c r="K21">
         <v>598.00157019999995</v>
       </c>
-      <c r="J21">
+      <c r="L21">
         <v>469.36370899999997</v>
       </c>
-      <c r="K21">
+      <c r="M21">
         <v>108.372</v>
       </c>
-      <c r="L21">
+      <c r="N21">
         <v>20.265999999999998</v>
       </c>
-      <c r="S21">
+      <c r="U21">
         <v>3.1</v>
       </c>
-      <c r="T21">
+      <c r="V21">
         <v>55</v>
       </c>
-      <c r="U21">
+      <c r="W21">
         <v>282.43</v>
       </c>
-      <c r="V21">
+      <c r="X21">
         <v>5.59</v>
       </c>
-      <c r="W21">
+      <c r="Y21">
         <v>2.83</v>
       </c>
-      <c r="Y21">
+      <c r="AA21">
         <v>3.24</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex3CvCrusher_TT</v>
@@ -1629,41 +1732,45 @@
       <c r="G22" s="1">
         <v>41515</v>
       </c>
-      <c r="H22">
-        <v>2013</v>
+      <c r="H22" s="3">
+        <f t="shared" si="1"/>
+        <v>128</v>
       </c>
       <c r="I22">
+        <v>2013</v>
+      </c>
+      <c r="K22">
         <v>362.10317179999998</v>
       </c>
-      <c r="J22">
+      <c r="L22">
         <v>259.64621529999999</v>
       </c>
-      <c r="K22">
+      <c r="M22">
         <v>82.484999999999999</v>
       </c>
-      <c r="L22">
+      <c r="N22">
         <v>19.972000000000001</v>
       </c>
-      <c r="S22">
+      <c r="U22">
         <v>2.23</v>
       </c>
-      <c r="T22">
+      <c r="V22">
         <v>44</v>
       </c>
-      <c r="U22">
+      <c r="W22">
         <v>271.61</v>
       </c>
-      <c r="V22">
+      <c r="X22">
         <v>6.17</v>
       </c>
-      <c r="W22">
+      <c r="Y22">
         <v>3.82</v>
       </c>
-      <c r="Y22">
+      <c r="AA22">
         <v>3.8</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex3CvHyola_575_CL_GT</v>
@@ -1686,41 +1793,45 @@
       <c r="G23" s="1">
         <v>41515</v>
       </c>
-      <c r="H23">
-        <v>2013</v>
+      <c r="H23" s="3">
+        <f t="shared" si="1"/>
+        <v>128</v>
       </c>
       <c r="I23">
+        <v>2013</v>
+      </c>
+      <c r="K23">
         <v>673.6989112</v>
       </c>
-      <c r="J23">
+      <c r="L23">
         <v>523.51197990000003</v>
       </c>
-      <c r="K23">
+      <c r="M23">
         <v>119.642</v>
       </c>
-      <c r="L23">
+      <c r="N23">
         <v>30.544</v>
       </c>
-      <c r="S23">
+      <c r="U23">
         <v>3.15</v>
       </c>
-      <c r="T23">
+      <c r="V23">
         <v>51</v>
       </c>
-      <c r="U23">
+      <c r="W23">
         <v>257.76</v>
       </c>
-      <c r="V23">
+      <c r="X23">
         <v>5.54</v>
       </c>
-      <c r="W23">
+      <c r="Y23">
         <v>2.88</v>
       </c>
-      <c r="Y23">
+      <c r="AA23">
         <v>3.23</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex3CvAV_Garnet</v>
@@ -1743,29 +1854,33 @@
       <c r="G24" s="1">
         <v>41543</v>
       </c>
-      <c r="H24">
-        <v>2013</v>
+      <c r="H24" s="3">
+        <f t="shared" si="1"/>
+        <v>156</v>
       </c>
       <c r="I24">
+        <v>2013</v>
+      </c>
+      <c r="K24">
         <v>1157.399476</v>
       </c>
-      <c r="J24">
+      <c r="L24">
         <v>666.00919999999996</v>
       </c>
-      <c r="K24">
+      <c r="M24">
         <v>35.551000000000002</v>
       </c>
-      <c r="L24">
-        <v>0</v>
-      </c>
-      <c r="S24">
-        <v>0</v>
-      </c>
-      <c r="T24">
+      <c r="N24">
+        <v>0</v>
+      </c>
+      <c r="U24">
+        <v>0</v>
+      </c>
+      <c r="V24">
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex3CvCrusher_TT</v>
@@ -1788,29 +1903,33 @@
       <c r="G25" s="1">
         <v>41543</v>
       </c>
-      <c r="H25">
-        <v>2013</v>
+      <c r="H25" s="3">
+        <f t="shared" si="1"/>
+        <v>156</v>
       </c>
       <c r="I25">
+        <v>2013</v>
+      </c>
+      <c r="K25">
         <v>745.24384239999995</v>
       </c>
-      <c r="J25">
+      <c r="L25">
         <v>422.53837709999999</v>
       </c>
-      <c r="K25">
+      <c r="M25">
         <v>37.972999999999999</v>
       </c>
-      <c r="L25">
-        <v>0</v>
-      </c>
-      <c r="S25">
-        <v>0</v>
-      </c>
-      <c r="T25">
+      <c r="N25">
+        <v>0</v>
+      </c>
+      <c r="U25">
+        <v>0</v>
+      </c>
+      <c r="V25">
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex3CvHyola_575_CL_GT</v>
@@ -1833,29 +1952,33 @@
       <c r="G26" s="1">
         <v>41543</v>
       </c>
-      <c r="H26">
-        <v>2013</v>
+      <c r="H26" s="3">
+        <f t="shared" si="1"/>
+        <v>156</v>
       </c>
       <c r="I26">
+        <v>2013</v>
+      </c>
+      <c r="K26">
         <v>1078.2827010000001</v>
       </c>
-      <c r="J26">
+      <c r="L26">
         <v>642.6608099</v>
       </c>
-      <c r="K26">
+      <c r="M26">
         <v>55.206000000000003</v>
       </c>
-      <c r="L26">
-        <v>0</v>
-      </c>
-      <c r="S26">
-        <v>0</v>
-      </c>
-      <c r="T26">
+      <c r="N26">
+        <v>0</v>
+      </c>
+      <c r="U26">
+        <v>0</v>
+      </c>
+      <c r="V26">
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex3CvAV_Garnet</v>
@@ -1878,50 +2001,57 @@
       <c r="G27" s="1">
         <v>41570</v>
       </c>
-      <c r="H27">
-        <v>2013</v>
+      <c r="H27" s="3">
+        <f t="shared" si="1"/>
+        <v>183</v>
       </c>
       <c r="I27">
+        <v>2013</v>
+      </c>
+      <c r="J27">
+        <v>9</v>
+      </c>
+      <c r="K27">
         <v>1140.9973299999999</v>
       </c>
-      <c r="J27">
+      <c r="L27">
         <v>457.08934870000002</v>
       </c>
-      <c r="K27">
-        <v>0</v>
-      </c>
-      <c r="L27">
-        <v>0</v>
-      </c>
       <c r="M27">
+        <v>0</v>
+      </c>
+      <c r="N27">
+        <v>0</v>
+      </c>
+      <c r="O27">
         <v>335.26600000000002</v>
       </c>
-      <c r="N27">
+      <c r="P27">
         <v>0.29099999999999998</v>
       </c>
-      <c r="O27">
+      <c r="Q27">
         <v>3.1709999999999998</v>
       </c>
-      <c r="P27">
+      <c r="R27">
         <v>3084.7750000000001</v>
       </c>
-      <c r="Q27">
+      <c r="S27">
         <v>105966.66800000001</v>
       </c>
-      <c r="R27">
+      <c r="T27">
         <v>34.64</v>
       </c>
-      <c r="S27">
-        <v>0</v>
-      </c>
-      <c r="T27">
+      <c r="U27">
+        <v>0</v>
+      </c>
+      <c r="V27">
         <v>41</v>
       </c>
-      <c r="X27">
+      <c r="Z27">
         <v>1.25</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex3CvCrusher_TT</v>
@@ -1944,50 +2074,57 @@
       <c r="G28" s="1">
         <v>41570</v>
       </c>
-      <c r="H28">
-        <v>2013</v>
+      <c r="H28" s="3">
+        <f t="shared" si="1"/>
+        <v>183</v>
       </c>
       <c r="I28">
+        <v>2013</v>
+      </c>
+      <c r="J28">
+        <v>9</v>
+      </c>
+      <c r="K28">
         <v>803.21128910000004</v>
       </c>
-      <c r="J28">
+      <c r="L28">
         <v>375.06271700000002</v>
       </c>
-      <c r="K28">
-        <v>0</v>
-      </c>
-      <c r="L28">
-        <v>0</v>
-      </c>
       <c r="M28">
+        <v>0</v>
+      </c>
+      <c r="N28">
+        <v>0</v>
+      </c>
+      <c r="O28">
         <v>209.84899999999999</v>
       </c>
-      <c r="N28">
+      <c r="P28">
         <v>0.26200000000000001</v>
       </c>
-      <c r="O28">
+      <c r="Q28">
         <v>2.79</v>
       </c>
-      <c r="P28">
+      <c r="R28">
         <v>2193.924493</v>
       </c>
-      <c r="Q28">
+      <c r="S28">
         <v>76401.240489999996</v>
       </c>
-      <c r="R28">
+      <c r="T28">
         <v>35.329523569999999</v>
       </c>
-      <c r="S28">
-        <v>0</v>
-      </c>
-      <c r="T28">
+      <c r="U28">
+        <v>0</v>
+      </c>
+      <c r="V28">
         <v>36</v>
       </c>
-      <c r="X28">
+      <c r="Z28">
         <v>1.44</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
         <f t="shared" si="0"/>
         <v>Greenethorpe2013_Ex3CvHyola_575_CL_GT</v>
@@ -2010,46 +2147,53 @@
       <c r="G29" s="1">
         <v>41570</v>
       </c>
-      <c r="H29">
-        <v>2013</v>
+      <c r="H29" s="3">
+        <f t="shared" si="1"/>
+        <v>183</v>
       </c>
       <c r="I29">
+        <v>2013</v>
+      </c>
+      <c r="J29">
+        <v>9</v>
+      </c>
+      <c r="K29">
         <v>1336.9879860000001</v>
       </c>
-      <c r="J29">
+      <c r="L29">
         <v>657.72001049999994</v>
       </c>
-      <c r="K29">
-        <v>0</v>
-      </c>
-      <c r="L29">
-        <v>0</v>
-      </c>
       <c r="M29">
+        <v>0</v>
+      </c>
+      <c r="N29">
+        <v>0</v>
+      </c>
+      <c r="O29">
         <v>329.7</v>
       </c>
-      <c r="N29">
+      <c r="P29">
         <v>0.245</v>
       </c>
-      <c r="O29">
+      <c r="Q29">
         <v>3.42</v>
       </c>
-      <c r="P29">
+      <c r="R29">
         <v>4279.2039999999997</v>
       </c>
-      <c r="Q29">
+      <c r="S29">
         <v>95862.459000000003</v>
       </c>
-      <c r="R29">
+      <c r="T29">
         <v>22.439</v>
       </c>
-      <c r="S29">
-        <v>0</v>
-      </c>
-      <c r="T29">
+      <c r="U29">
+        <v>0</v>
+      </c>
+      <c r="V29">
         <v>41</v>
       </c>
-      <c r="X29">
+      <c r="Z29">
         <v>1.02</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated phenology runs and observed file
updated OCP phenology data, draft of Genomics runs
</commit_message>
<xml_diff>
--- a/Prototypes/Canola/Greenethorpe2013.xlsx
+++ b/Prototypes/Canola/Greenethorpe2013.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lil026\ApsimX\Prototypes\Canola\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A35AD16-7C21-4BBF-A88B-83BC288628E0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABC5A9ED-3A3F-4BF5-BCCD-16633FC4D25D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{82FDB4BE-E74B-4488-8680-42A462D2A87F}"/>
+    <workbookView xWindow="8595" yWindow="2280" windowWidth="26295" windowHeight="13095" xr2:uid="{82FDB4BE-E74B-4488-8680-42A462D2A87F}"/>
   </bookViews>
   <sheets>
     <sheet name="Observed" sheetId="1" r:id="rId1"/>
@@ -129,9 +129,6 @@
     <t>Canola.Stem.Wt</t>
   </si>
   <si>
-    <t>Canola.Cultivar</t>
-  </si>
-  <si>
     <t>Canola.Grain.Wt</t>
   </si>
   <si>
@@ -160,6 +157,9 @@
   </si>
   <si>
     <t>Hyola575_CL</t>
+  </si>
+  <si>
+    <t>Cv</t>
   </si>
 </sst>
 </file>
@@ -517,7 +517,7 @@
   <dimension ref="A1:AA29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -562,7 +562,7 @@
         <v>21</v>
       </c>
       <c r="D1" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="E1" t="s">
         <v>20</v>
@@ -574,13 +574,13 @@
         <v>18</v>
       </c>
       <c r="H1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I1" t="s">
         <v>17</v>
       </c>
       <c r="J1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K1" t="s">
         <v>16</v>
@@ -595,19 +595,19 @@
         <v>14</v>
       </c>
       <c r="O1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P1" t="s">
         <v>13</v>
       </c>
       <c r="Q1" t="s">
+        <v>26</v>
+      </c>
+      <c r="R1" t="s">
         <v>27</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>28</v>
-      </c>
-      <c r="S1" t="s">
-        <v>29</v>
       </c>
       <c r="T1" t="s">
         <v>12</v>
@@ -616,10 +616,10 @@
         <v>11</v>
       </c>
       <c r="V1" t="s">
+        <v>29</v>
+      </c>
+      <c r="W1" t="s">
         <v>30</v>
-      </c>
-      <c r="W1" t="s">
-        <v>31</v>
       </c>
       <c r="X1" t="s">
         <v>10</v>
@@ -628,7 +628,7 @@
         <v>9</v>
       </c>
       <c r="Z1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AA1" t="s">
         <v>8</v>
@@ -1019,7 +1019,7 @@
         <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E9" t="s">
         <v>0</v>
@@ -1053,7 +1053,7 @@
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E10" t="s">
         <v>0</v>
@@ -1105,7 +1105,7 @@
         <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E11" t="s">
         <v>0</v>
@@ -1157,7 +1157,7 @@
         <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E12" t="s">
         <v>0</v>
@@ -1209,7 +1209,7 @@
         <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E13" t="s">
         <v>0</v>
@@ -1261,7 +1261,7 @@
         <v>5</v>
       </c>
       <c r="D14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E14" t="s">
         <v>0</v>
@@ -1435,7 +1435,7 @@
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E17" t="s">
         <v>0</v>
@@ -1603,7 +1603,7 @@
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E20" t="s">
         <v>0</v>
@@ -1783,7 +1783,7 @@
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E23" t="s">
         <v>0</v>
@@ -1942,7 +1942,7 @@
         <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E26" t="s">
         <v>0</v>
@@ -2137,7 +2137,7 @@
         <v>1</v>
       </c>
       <c r="D29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E29" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
Updated obs files using CSV to remove excel cell formatting and graphs in apsimx file
</commit_message>
<xml_diff>
--- a/Prototypes/Canola/Greenethorpe2013.xlsx
+++ b/Prototypes/Canola/Greenethorpe2013.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lil026\ApsimX\Prototypes\Canola\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABC5A9ED-3A3F-4BF5-BCCD-16633FC4D25D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79AF2F52-79F4-49C3-BF80-7DAD171CA355}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8595" yWindow="2280" windowWidth="26295" windowHeight="13095" xr2:uid="{82FDB4BE-E74B-4488-8680-42A462D2A87F}"/>
+    <workbookView xWindow="13170" yWindow="8280" windowWidth="24420" windowHeight="13095" xr2:uid="{82FDB4BE-E74B-4488-8680-42A462D2A87F}"/>
   </bookViews>
   <sheets>
     <sheet name="Observed" sheetId="1" r:id="rId1"/>
@@ -105,21 +105,12 @@
     <t>Canola.AboveGround.Wt</t>
   </si>
   <si>
-    <t>Clock.Today.Year</t>
-  </si>
-  <si>
     <t>Clock.Today</t>
   </si>
   <si>
-    <t>Canola.SowingDate</t>
-  </si>
-  <si>
     <t>treat</t>
   </si>
   <si>
-    <t>exp</t>
-  </si>
-  <si>
     <t>site</t>
   </si>
   <si>
@@ -160,6 +151,15 @@
   </si>
   <si>
     <t>Cv</t>
+  </si>
+  <si>
+    <t>exp_no</t>
+  </si>
+  <si>
+    <t>SowingDate</t>
+  </si>
+  <si>
+    <t>Year</t>
   </si>
 </sst>
 </file>
@@ -517,7 +517,7 @@
   <dimension ref="A1:AA29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,40 +553,40 @@
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C1" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="D1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" t="s">
         <v>35</v>
       </c>
-      <c r="E1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I1" t="s">
-        <v>17</v>
-      </c>
       <c r="J1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="K1" t="s">
         <v>16</v>
       </c>
       <c r="L1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="M1" t="s">
         <v>15</v>
@@ -595,19 +595,19 @@
         <v>14</v>
       </c>
       <c r="O1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="P1" t="s">
         <v>13</v>
       </c>
       <c r="Q1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="R1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="S1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="T1" t="s">
         <v>12</v>
@@ -616,10 +616,10 @@
         <v>11</v>
       </c>
       <c r="V1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="W1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="X1" t="s">
         <v>10</v>
@@ -628,7 +628,7 @@
         <v>9</v>
       </c>
       <c r="Z1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="AA1" t="s">
         <v>8</v>
@@ -1019,7 +1019,7 @@
         <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E9" t="s">
         <v>0</v>
@@ -1053,7 +1053,7 @@
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E10" t="s">
         <v>0</v>
@@ -1105,7 +1105,7 @@
         <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E11" t="s">
         <v>0</v>
@@ -1157,7 +1157,7 @@
         <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E12" t="s">
         <v>0</v>
@@ -1209,7 +1209,7 @@
         <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E13" t="s">
         <v>0</v>
@@ -1261,7 +1261,7 @@
         <v>5</v>
       </c>
       <c r="D14" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E14" t="s">
         <v>0</v>
@@ -1435,7 +1435,7 @@
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E17" t="s">
         <v>0</v>
@@ -1603,7 +1603,7 @@
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E20" t="s">
         <v>0</v>
@@ -1783,7 +1783,7 @@
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E23" t="s">
         <v>0</v>
@@ -1942,7 +1942,7 @@
         <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E26" t="s">
         <v>0</v>
@@ -2137,7 +2137,7 @@
         <v>1</v>
       </c>
       <c r="D29" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E29" t="s">
         <v>0</v>

</xml_diff>